<commit_message>
3 dimension sim and year on same plot
</commit_message>
<xml_diff>
--- a/input_variables_list/Manage_input_variables_list_IDN_v00.xlsx
+++ b/input_variables_list/Manage_input_variables_list_IDN_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="98">
   <si>
     <t>variable_name</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>Services</t>
+  </si>
+  <si>
+    <t>Aggregate labor supply</t>
+  </si>
+  <si>
+    <t>2025, 2030</t>
+  </si>
+  <si>
+    <t>lsT</t>
   </si>
 </sst>
 </file>
@@ -797,13 +806,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,30 +1151,30 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
@@ -1179,7 +1188,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1190,14 +1199,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
@@ -1402,7 +1411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1605,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1715,6 +1724,23 @@
       </c>
       <c r="G5">
         <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1953,13 +1979,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>